<commit_message>
masih kurang banyak nar
</commit_message>
<xml_diff>
--- a/excel/import invoice.xlsx
+++ b/excel/import invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/fa_sai/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8104DB51-5581-2F49-B11F-6C5F2452B4C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8021FA1-9CCA-1840-9020-6E3655AC27CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{9FD7B6F2-6130-294A-869E-9040C2B0795A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
   <si>
     <t>Invoice Number</t>
   </si>
@@ -106,6 +106,174 @@
   </si>
   <si>
     <t>98,07</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>7194-3042-30</t>
+  </si>
+  <si>
+    <t>FMTH</t>
+  </si>
+  <si>
+    <t>RM01-1711</t>
+  </si>
+  <si>
+    <t>7194-3323-30</t>
+  </si>
+  <si>
+    <t>270</t>
+  </si>
+  <si>
+    <t>JL01-8173</t>
+  </si>
+  <si>
+    <t>7173-1696-10</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>730</t>
+  </si>
+  <si>
+    <t>RM01-1880</t>
+  </si>
+  <si>
+    <t>PT. NANBU PLASTICS I</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>7173-1919</t>
+  </si>
+  <si>
+    <t>JL03-8022</t>
+  </si>
+  <si>
+    <t>7173-2329</t>
+  </si>
+  <si>
+    <t>JL03-8023</t>
+  </si>
+  <si>
+    <t>5500</t>
+  </si>
+  <si>
+    <t>7173-2464-30</t>
+  </si>
+  <si>
+    <t>JL03-8024</t>
+  </si>
+  <si>
+    <t>PT. PIOLAX INDONESIA</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>60,1</t>
+  </si>
+  <si>
+    <t>88,7</t>
+  </si>
+  <si>
+    <t>7189-8974-30</t>
+  </si>
+  <si>
+    <t>20,9</t>
+  </si>
+  <si>
+    <t>701</t>
+  </si>
+  <si>
+    <t>7189-8974-90</t>
+  </si>
+  <si>
+    <t>ARROW ELECTRONICS AS</t>
+  </si>
+  <si>
+    <t>880</t>
+  </si>
+  <si>
+    <t>89,7</t>
+  </si>
+  <si>
+    <t>HELLERMANN TYTON</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>78,98</t>
+  </si>
+  <si>
+    <t>10100</t>
+  </si>
+  <si>
+    <t>780</t>
+  </si>
+  <si>
+    <t>JL03-8025</t>
+  </si>
+  <si>
+    <t>JL03-8026</t>
+  </si>
+  <si>
+    <t>JL03-8027</t>
+  </si>
+  <si>
+    <t>JL03-8028</t>
+  </si>
+  <si>
+    <t>7194-3003-30</t>
+  </si>
+  <si>
+    <t>7173-2783-30</t>
+  </si>
+  <si>
+    <t>7173-0417-52</t>
+  </si>
+  <si>
+    <t>7173-2330</t>
+  </si>
+  <si>
+    <t>JL03-8029</t>
+  </si>
+  <si>
+    <t>JL03-8030</t>
+  </si>
+  <si>
+    <t>JL03-8031</t>
+  </si>
+  <si>
+    <t>781</t>
+  </si>
+  <si>
+    <t>782</t>
+  </si>
+  <si>
+    <t>783</t>
+  </si>
+  <si>
+    <t>NIFCO</t>
+  </si>
+  <si>
+    <t>PT. CATURINDO AGUNG</t>
+  </si>
+  <si>
+    <t>78,99</t>
+  </si>
+  <si>
+    <t>78,100</t>
+  </si>
+  <si>
+    <t>78,101</t>
   </si>
 </sst>
 </file>
@@ -115,7 +283,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,6 +301,26 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cilibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Cilibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -181,17 +369,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -218,6 +399,53 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,369 +761,1042 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD29480-4CCB-694E-9DE3-D08F756A8C73}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:AC50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="18"/>
+    <col min="2" max="2" width="11.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" style="18"/>
+    <col min="7" max="7" width="19.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="28" width="10.83203125" style="18"/>
+    <col min="29" max="29" width="18.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:29">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:29" s="4" customFormat="1">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="10">
         <v>43593</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="11">
         <v>200</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="11">
         <v>71.739999999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:29" s="4" customFormat="1">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>43593</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="11">
         <v>17600</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:29" s="4" customFormat="1">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="10">
         <v>43525</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <v>1500</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="11">
         <v>81.19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:29" s="4" customFormat="1">
+      <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="10">
         <v>43770</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="11">
         <v>1000</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="11">
         <v>81.19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:29" s="4" customFormat="1">
+      <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="10">
         <v>43709</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <v>600</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="11">
         <v>81.38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:29" s="4" customFormat="1">
+      <c r="A7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="13">
         <v>43483</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="14">
         <v>540</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="14">
         <v>322.11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:29" s="4" customFormat="1">
+      <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="13">
         <v>43483</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="14">
         <v>5000</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="14">
+        <v>81.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" s="4" customFormat="1">
+      <c r="A9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="13">
+        <v>43658</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="14">
+        <v>4000</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14">
         <v>81.19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="16">
-        <v>43658</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="17">
-        <v>4000</v>
-      </c>
-      <c r="E9" s="14" t="s">
+    <row r="10" spans="1:29" s="4" customFormat="1">
+      <c r="A10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="13">
+        <v>43499</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="14">
+        <v>500</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="14">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" s="17" customFormat="1">
+      <c r="A11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="16">
+        <v>43564</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="22"/>
+    </row>
+    <row r="12" spans="1:29" s="17" customFormat="1">
+      <c r="A12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="16">
+        <v>43748</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="22"/>
+    </row>
+    <row r="13" spans="1:29" s="17" customFormat="1">
+      <c r="A13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="16">
+        <v>43627</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="20"/>
+      <c r="AA13" s="20"/>
+      <c r="AB13" s="20"/>
+      <c r="AC13" s="22"/>
+    </row>
+    <row r="14" spans="1:29" s="19" customFormat="1">
+      <c r="A14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="16">
+        <v>43728</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="17">
-        <v>81.19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:7" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="20"/>
+      <c r="AA14" s="20"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="22"/>
+    </row>
+    <row r="15" spans="1:29" s="19" customFormat="1">
+      <c r="A15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="16">
+        <v>43486</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="20"/>
+      <c r="Z15" s="20"/>
+      <c r="AA15" s="20"/>
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="22"/>
+    </row>
+    <row r="16" spans="1:29" s="19" customFormat="1">
+      <c r="A16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="16">
+        <v>43458</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
+      <c r="AA16" s="20"/>
+      <c r="AB16" s="20"/>
+      <c r="AC16" s="22"/>
+    </row>
+    <row r="17" spans="1:29" s="19" customFormat="1">
+      <c r="A17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="16">
+        <v>43449</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="22"/>
+    </row>
+    <row r="18" spans="1:29">
+      <c r="A18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="10">
+        <v>43597</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23"/>
+      <c r="Z18" s="23"/>
+      <c r="AA18" s="23"/>
+      <c r="AB18" s="23"/>
+      <c r="AC18" s="23"/>
+    </row>
+    <row r="19" spans="1:29">
+      <c r="A19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="28">
+        <v>43601</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23"/>
+    </row>
+    <row r="20" spans="1:29">
+      <c r="A20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="10">
+        <v>43694</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="23"/>
+    </row>
+    <row r="21" spans="1:29">
+      <c r="A21" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="10">
+        <v>43736</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="23"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="23"/>
+    </row>
+    <row r="22" spans="1:29">
+      <c r="A22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="10">
+        <v>43788</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="25"/>
+    </row>
+    <row r="23" spans="1:29">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="25"/>
+    </row>
+    <row r="24" spans="1:29">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="25"/>
+    </row>
+    <row r="25" spans="1:29" s="25" customFormat="1">
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="31"/>
+      <c r="W25" s="31"/>
+      <c r="X25" s="31"/>
+      <c r="Y25" s="31"/>
+      <c r="Z25" s="31"/>
+      <c r="AA25" s="31"/>
+      <c r="AB25" s="31"/>
+      <c r="AC25" s="32"/>
+    </row>
+    <row r="26" spans="1:29" s="25" customFormat="1">
+      <c r="A26" s="33"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="31"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="31"/>
+      <c r="W26" s="31"/>
+      <c r="X26" s="31"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="31"/>
+      <c r="AA26" s="31"/>
+      <c r="AB26" s="31"/>
+      <c r="AC26" s="32"/>
+    </row>
+    <row r="27" spans="1:29" s="23" customFormat="1">
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="31"/>
+      <c r="X27" s="31"/>
+      <c r="Y27" s="31"/>
+      <c r="Z27" s="31"/>
+      <c r="AA27" s="31"/>
+      <c r="AB27" s="31"/>
+      <c r="AC27" s="32"/>
+    </row>
+    <row r="28" spans="1:29" s="23" customFormat="1">
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="31"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="31"/>
+      <c r="S28" s="31"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="31"/>
+      <c r="V28" s="31"/>
+      <c r="W28" s="31"/>
+      <c r="X28" s="31"/>
+      <c r="Y28" s="31"/>
+      <c r="Z28" s="31"/>
+      <c r="AA28" s="31"/>
+      <c r="AB28" s="31"/>
+      <c r="AC28" s="32"/>
+    </row>
+    <row r="29" spans="1:29" s="23" customFormat="1">
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="31"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="31"/>
+      <c r="W29" s="31"/>
+      <c r="X29" s="31"/>
+      <c r="Y29" s="31"/>
+      <c r="Z29" s="31"/>
+      <c r="AA29" s="31"/>
+      <c r="AB29" s="31"/>
+      <c r="AC29" s="32"/>
+    </row>
+    <row r="30" spans="1:29" s="23" customFormat="1">
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="31"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="31"/>
+      <c r="X30" s="31"/>
+      <c r="Y30" s="31"/>
+      <c r="Z30" s="31"/>
+      <c r="AA30" s="31"/>
+      <c r="AB30" s="31"/>
+      <c r="AC30" s="32"/>
+    </row>
+    <row r="31" spans="1:29">
       <c r="A31" s="1"/>
       <c r="B31" s="3"/>
       <c r="C31" s="2"/>
@@ -904,7 +1805,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29">
       <c r="A32" s="1"/>
       <c r="B32" s="3"/>
       <c r="C32" s="2"/>
@@ -913,7 +1814,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="1"/>
       <c r="B33" s="3"/>
       <c r="C33" s="2"/>
@@ -922,7 +1823,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="2"/>
@@ -931,7 +1832,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="1"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2"/>
@@ -940,7 +1841,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="1"/>
       <c r="B36" s="3"/>
       <c r="C36" s="2"/>
@@ -949,7 +1850,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="1"/>
       <c r="B37" s="3"/>
       <c r="C37" s="2"/>
@@ -958,7 +1859,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="1"/>
       <c r="B38" s="3"/>
       <c r="C38" s="2"/>
@@ -967,7 +1868,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="1"/>
       <c r="B39" s="3"/>
       <c r="C39" s="2"/>
@@ -976,7 +1877,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="1"/>
       <c r="B40" s="3"/>
       <c r="C40" s="2"/>
@@ -985,7 +1886,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="1"/>
       <c r="B41" s="3"/>
       <c r="C41" s="2"/>
@@ -994,7 +1895,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="1"/>
       <c r="B42" s="3"/>
       <c r="C42" s="2"/>
@@ -1003,7 +1904,7 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="1"/>
       <c r="B43" s="3"/>
       <c r="C43" s="2"/>
@@ -1012,7 +1913,7 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="1"/>
       <c r="B44" s="3"/>
       <c r="C44" s="2"/>
@@ -1021,7 +1922,7 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="1"/>
       <c r="B45" s="3"/>
       <c r="C45" s="2"/>
@@ -1030,7 +1931,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="1"/>
       <c r="B46" s="3"/>
       <c r="C46" s="2"/>
@@ -1039,7 +1940,7 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="1"/>
       <c r="B47" s="3"/>
       <c r="C47" s="2"/>
@@ -1048,7 +1949,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="1"/>
       <c r="B48" s="3"/>
       <c r="C48" s="2"/>
@@ -1057,7 +1958,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" s="1"/>
       <c r="B49" s="3"/>
       <c r="C49" s="2"/>
@@ -1066,7 +1967,7 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" s="1"/>
       <c r="B50" s="3"/>
       <c r="C50" s="2"/>

</xml_diff>

<commit_message>
Alhamdulillah besok demo hee
</commit_message>
<xml_diff>
--- a/excel/import invoice.xlsx
+++ b/excel/import invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/fa_sai/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF0C1C8-F6E4-624F-9F98-ED8BE362D176}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0113AB9-3FEF-D24A-8AC1-8A03F8A4383D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14060" xr2:uid="{329E2B7B-EBAD-E649-85EA-0820AD4453A7}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="73">
   <si>
     <t>HIB</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>SCHLEMMER2</t>
+  </si>
+  <si>
+    <t>TAP</t>
   </si>
 </sst>
 </file>
@@ -285,7 +288,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -348,6 +351,12 @@
       <color rgb="FF333333"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="High Tower Text"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -416,7 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -452,6 +461,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,11 +781,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5931E9C3-C962-3846-B590-0F2E86192E67}">
   <dimension ref="A1:AC26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
@@ -781,7 +793,7 @@
     <col min="22" max="22" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -870,7 +882,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -925,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -980,7 +992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1035,7 +1047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1090,7 +1102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1145,7 +1157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1200,7 +1212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1255,7 +1267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1310,7 +1322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1365,7 +1377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1420,7 +1432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1475,7 +1487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1530,7 +1542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1585,7 +1597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1640,7 +1652,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1695,7 +1707,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1750,7 +1762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1805,7 +1817,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1860,7 +1872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1915,7 +1927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1970,7 +1982,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -2018,14 +2030,14 @@
       <c r="U22" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="V22" s="6" t="s">
-        <v>0</v>
+      <c r="V22" s="17" t="s">
+        <v>72</v>
       </c>
       <c r="W22" s="5">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -2080,7 +2092,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -2135,7 +2147,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -2190,7 +2202,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" ht="18">
       <c r="A26" s="5">
         <v>25</v>
       </c>

</xml_diff>